<commit_message>
wet lab not allowed to create pseudo samples and libs
</commit_message>
<xml_diff>
--- a/db/template.xlsx
+++ b/db/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liyuxin/Dropbox/Yuxin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liyuxin/djangoprojects/epigen_ucsd_django/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4373A597-5384-8F4C-91F9-53621BD7A2A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970E7D3F-E84D-0E4E-9EB4-A2B75D459F52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="2820" windowWidth="48900" windowHeight="22460" xr2:uid="{0BA43C7A-E819-E44A-BC5D-1B0EA814106C}"/>
+    <workbookView xWindow="2620" yWindow="3180" windowWidth="48900" windowHeight="22460" xr2:uid="{0BA43C7A-E819-E44A-BC5D-1B0EA814106C}"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" r:id="rId1"/>
@@ -30,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="94">
   <si>
     <t>From sample submission form</t>
   </si>
   <si>
-    <t>sample ID (copied from column I)</t>
-  </si>
-  <si>
     <t>To be entered upon reciept</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Storage location</t>
   </si>
   <si>
-    <t>sample ID (from LIMS if available)</t>
-  </si>
-  <si>
     <t>Library description</t>
   </si>
   <si>
@@ -315,6 +309,9 @@
   </si>
   <si>
     <t>used up</t>
+  </si>
+  <si>
+    <t>Sample ID (Must Match Column I in Sample Sheet)</t>
   </si>
 </sst>
 </file>
@@ -411,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -466,32 +463,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -501,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -511,28 +482,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7609B9-C4B6-F14F-A209-FF45D69C71CA}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -874,14 +840,13 @@
     <col min="19" max="19" width="14.1640625" customWidth="1"/>
     <col min="20" max="20" width="13.33203125" customWidth="1"/>
     <col min="21" max="21" width="45.1640625" customWidth="1"/>
-    <col min="22" max="22" width="15.5" customWidth="1"/>
-    <col min="23" max="23" width="14.1640625" customWidth="1"/>
-    <col min="24" max="24" width="14" customWidth="1"/>
-    <col min="25" max="25" width="11.83203125" customWidth="1"/>
-    <col min="26" max="26" width="43.33203125" customWidth="1"/>
+    <col min="22" max="22" width="14.1640625" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
+    <col min="24" max="24" width="11.83203125" customWidth="1"/>
+    <col min="25" max="25" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -905,100 +870,93 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="5"/>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="8"/>
+    </row>
+    <row r="2" spans="1:25" ht="46" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="8"/>
-    </row>
-    <row r="2" spans="1:26" ht="46" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="P2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="R2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="S2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="T2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="U2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="22"/>
       <c r="W2" s="10" t="s">
         <v>24</v>
       </c>
       <c r="X2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z2" s="9" t="s">
-        <v>23</v>
+      <c r="Y2" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="V1:V2"/>
-  </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576 W3:W1048576" xr:uid="{2E778634-3350-3242-8614-54899DD376E9}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576 V3:V1048576" xr:uid="{2E778634-3350-3242-8614-54899DD376E9}">
       <formula1>42736</formula1>
     </dataValidation>
   </dataValidations>
@@ -1058,7 +1016,7 @@
           <x14:formula1>
             <xm:f>samples_validation!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Y3:Y1048576</xm:sqref>
+          <xm:sqref>X3:X1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE30D4AF-4A47-1240-A444-C0EDDC356808}">
           <x14:formula1>
@@ -1076,13 +1034,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FDDB9A-F01E-4849-87EC-00E3C8EFF76F}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
@@ -1094,34 +1050,34 @@
   <sheetData>
     <row r="1" spans="1:15" ht="43" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="J1" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K1" s="15"/>
       <c r="L1" s="16"/>
@@ -1156,12 +1112,12 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" customWidth="1"/>
@@ -1178,52 +1134,52 @@
   <sheetData>
     <row r="1" spans="1:16" ht="29" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="J1" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="L1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>84</v>
-      </c>
       <c r="P1" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1284,162 +1240,162 @@
   <sheetData>
     <row r="1" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>20</v>
-      </c>
       <c r="H1" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>54</v>
-      </c>
       <c r="F2" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>55</v>
-      </c>
       <c r="F3" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>49</v>
-      </c>
       <c r="E4" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
@@ -1448,7 +1404,7 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="F7" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
@@ -4455,57 +4411,57 @@
   <sheetData>
     <row r="1" spans="1:1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -7502,102 +7458,102 @@
   <sheetData>
     <row r="1" spans="1:4" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify template a little bit
</commit_message>
<xml_diff>
--- a/db/template.xlsx
+++ b/db/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liyuxin/djangoprojects/epigen_ucsd_django/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970E7D3F-E84D-0E4E-9EB4-A2B75D459F52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454578F5-A201-D047-8971-4F5C65FCEB7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="3180" windowWidth="48900" windowHeight="22460" xr2:uid="{0BA43C7A-E819-E44A-BC5D-1B0EA814106C}"/>
+    <workbookView xWindow="2300" yWindow="3180" windowWidth="48900" windowHeight="22460" xr2:uid="{0BA43C7A-E819-E44A-BC5D-1B0EA814106C}"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>From sample submission form</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>Sample ID (Must Match Column I in Sample Sheet)</t>
+  </si>
+  <si>
+    <t>Internal Notes</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,7 +954,7 @@
         <v>25</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>